<commit_message>
Added Nvidia Jetson Results
</commit_message>
<xml_diff>
--- a/Benchmark_results.xlsx
+++ b/Benchmark_results.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
-  <workbookPr date1904="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lstm-research\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0042761B-A946-44A3-9D0F-E9C75261C55E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="13680" windowHeight="5210"/>
+    <workbookView xWindow="5175" yWindow="2265" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark_results.csv" sheetId="1" r:id="rId1"/>
@@ -13,13 +19,13 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Sheet_Title" localSheetId="0">"Benchmark_results.csv"</definedName>
   </definedNames>
-  <calcPr calcMode="auto" iterate="1" iterateCount="100" iterateDelta="0.001"/>
-  <webPublishing allowPng="1" css="0" codePage="1252"/>
+  <calcPr calcId="0" iterate="1"/>
+  <webPublishing css="0" allowPng="1" codePage="1252"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41" count="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="52">
   <si>
     <t>Accuracy</t>
   </si>
@@ -142,25 +148,50 @@
   </si>
   <si>
     <t>Kemal 1300hz</t>
+  </si>
+  <si>
+    <t>Tensorflow Full</t>
+  </si>
+  <si>
+    <t>Tensorflow Lite Testing Data</t>
+  </si>
+  <si>
+    <t>Tensorflow Lite Kemal 360hz</t>
+  </si>
+  <si>
+    <t>Tensorflow Lite Kemal 500hz</t>
+  </si>
+  <si>
+    <t>Tensorflow Lite Kemal 1300hz</t>
+  </si>
+  <si>
+    <t>Time per record [Seconds]</t>
+  </si>
+  <si>
+    <t>Time per record[S]</t>
+  </si>
+  <si>
+    <t>Ryzen 5 3600</t>
+  </si>
+  <si>
+    <t>Jetson Nano CPU</t>
+  </si>
+  <si>
+    <t>Nvidia Jetson Nano</t>
+  </si>
+  <si>
+    <t>D-90-L45 MIT-18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="m/d/yyyy" numFmtId="100"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <u val="none"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
-      <vertAlign val="baseline"/>
-      <sz val="10"/>
-      <strike val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,99 +203,375 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="0" diagonalDown="0">
-      <left style="none">
-        <color rgb="FFC7C7C7"/>
-      </left>
-      <right style="none">
-        <color rgb="FFC7C7C7"/>
-      </right>
-      <top style="none">
-        <color rgb="FFC7C7C7"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FFC7C7C7"/>
-      </bottom>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" numFmtId="100" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="0" shrinkToFit="0" textRotation="0" indent="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:gnmx="http://www.gnumeric.org/ext/spreadsheetml">
-  <sheetPr>
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
-  <dimension ref="A1:V28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V36"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" style="0" width="16.28473557692308" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" style="0" width="9.142307692307693"/>
-    <col min="4" max="4" style="0" width="22.57007211538462" bestFit="1" customWidth="1"/>
-    <col min="5" max="256" style="0" width="9.142307692307693"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Tensorflow Full</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Tensorflow Lite Testing Data</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Tensorflow Lite Kemal 360hz</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Tensorflow Lite Kemal 500hz</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Tensorflow Lite Kemal 1300hz</t>
-        </is>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Time per record [Seconds]</t>
-        </is>
+      <c r="F2" t="s">
+        <v>46</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Time per record[S]</t>
-        </is>
+      <c r="H2" t="s">
+        <v>47</v>
       </c>
       <c r="I2" t="s">
         <v>1</v>
@@ -295,49 +602,47 @@
       </c>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Ryzen 5 3600</t>
-        </is>
+      <c r="A3" t="s">
+        <v>48</v>
       </c>
       <c r="E3">
-        <v>0.97999999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="F3">
-        <v>0.036990000000000002</v>
+        <v>3.6990000000000002E-2</v>
       </c>
       <c r="G3">
-        <v>0.97999999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="H3">
-        <v>0.0033999999999999998</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>0.0033</v>
+        <v>3.3E-3</v>
       </c>
       <c r="K3">
-        <v>0.0027000000000000001</v>
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="L3">
-        <v>0.98999999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="M3">
-        <v>0.0033999999999999998</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="N3">
-        <v>0.0020999999999999999</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3">
-        <v>0.0037000000000000002</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="Q3">
-        <v>0.0022000000000000001</v>
+        <v>2.2000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -351,37 +656,37 @@
         <v>5</v>
       </c>
       <c r="G4">
-        <v>0.97999999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="H4">
-        <v>0.017000000000000001</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
-        <v>0.017100000000000001</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="K4">
-        <v>0.013690000000000001</v>
+        <v>1.3690000000000001E-2</v>
       </c>
       <c r="L4">
-        <v>0.98999999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="M4">
-        <v>0.017299999999999999</v>
+        <v>1.7299999999999999E-2</v>
       </c>
       <c r="N4">
-        <v>0.012999999999999999</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="O4">
         <v>1</v>
       </c>
       <c r="P4">
-        <v>0.0172</v>
+        <v>1.72E-2</v>
       </c>
       <c r="Q4">
-        <v>0.01337</v>
+        <v>1.337E-2</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -395,17 +700,15 @@
         <v>5</v>
       </c>
       <c r="G5">
-        <v>0.97999999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="H5">
-        <v>0.048800000000000003</v>
+        <v>4.8800000000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Jetson Nano CPU</t>
-        </is>
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -414,103 +717,47 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>0.97999999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="H6">
-        <v>0.0184</v>
+        <v>1.84E-2</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0.0184</v>
+        <v>1.84E-2</v>
       </c>
       <c r="K6">
-        <v>0.015900000000000001</v>
+        <v>1.5900000000000001E-2</v>
       </c>
       <c r="L6">
-        <v>0.98999999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="M6">
-        <v>0.0189</v>
+        <v>1.89E-2</v>
       </c>
       <c r="N6">
-        <v>0.0137</v>
+        <v>1.37E-2</v>
       </c>
       <c r="O6">
         <v>1</v>
       </c>
       <c r="P6">
-        <v>0.018499999999999999</v>
+        <v>1.8499999999999999E-2</v>
       </c>
       <c r="Q6">
-        <v>0.0135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" t="s">
-        <v>4</v>
+        <v>1.35E-2</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" t="s">
-        <v>15</v>
-      </c>
-      <c r="M13" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" t="s">
-        <v>17</v>
-      </c>
-      <c r="O13" t="s">
-        <v>18</v>
-      </c>
-      <c r="P13" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>20</v>
-      </c>
-      <c r="R13" t="s">
-        <v>21</v>
-      </c>
-      <c r="S13" t="s">
-        <v>22</v>
-      </c>
-      <c r="T13" t="s">
-        <v>23</v>
-      </c>
-      <c r="U13" t="s">
-        <v>24</v>
-      </c>
-      <c r="V13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -524,58 +771,58 @@
         <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>32</v>
-      </c>
-      <c r="J14" s="1">
-        <v>44379</v>
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="L14" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="O14" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="P14" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>44413</v>
+        <v>19</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>20</v>
       </c>
       <c r="R14" t="s">
-        <v>31</v>
-      </c>
-      <c r="S14" s="1">
-        <v>44258</v>
-      </c>
-      <c r="T14">
-        <v>91</v>
-      </c>
-      <c r="U14" s="1">
-        <v>44319</v>
+        <v>21</v>
+      </c>
+      <c r="S14" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" t="s">
+        <v>24</v>
       </c>
       <c r="V14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -583,13 +830,67 @@
         <v>36</v>
       </c>
       <c r="B15">
-        <v>0.96999999999999997</v>
+        <v>0.97</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15">
-        <v>0.025499999999999998</v>
+        <v>2.5499999999999998E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="1">
+        <v>44379</v>
+      </c>
+      <c r="K15" t="s">
+        <v>33</v>
+      </c>
+      <c r="L15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" t="s">
+        <v>31</v>
+      </c>
+      <c r="O15" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>44413</v>
+      </c>
+      <c r="R15" t="s">
+        <v>31</v>
+      </c>
+      <c r="S15" s="1">
+        <v>44258</v>
+      </c>
+      <c r="T15">
+        <v>91</v>
+      </c>
+      <c r="U15" s="1">
+        <v>44319</v>
+      </c>
+      <c r="V15" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -600,10 +901,10 @@
         <v>38</v>
       </c>
       <c r="C16">
-        <v>0.014120000000000001</v>
+        <v>1.4120000000000001E-2</v>
       </c>
       <c r="D16">
-        <v>0.026100000000000002</v>
+        <v>2.6100000000000002E-2</v>
       </c>
       <c r="E16">
         <v>67</v>
@@ -668,10 +969,10 @@
         <v>38</v>
       </c>
       <c r="C17">
-        <v>0.01324</v>
+        <v>1.324E-2</v>
       </c>
       <c r="D17">
-        <v>0.025499999999999998</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="E17">
         <v>68</v>
@@ -736,10 +1037,10 @@
         <v>38</v>
       </c>
       <c r="C18">
-        <v>0.01324</v>
+        <v>1.324E-2</v>
       </c>
       <c r="D18">
-        <v>0.025499999999999998</v>
+        <v>2.5499999999999998E-2</v>
       </c>
       <c r="E18">
         <v>73</v>
@@ -756,19 +1057,66 @@
       <c r="I18">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="13.5">
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="13.5">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="13.5">
-      <c r="B23"/>
+    <row r="23" spans="1:22">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
       <c r="E23" t="s">
         <v>8</v>
       </c>
@@ -824,15 +1172,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="13.5">
-      <c r="B24" t="s">
-        <v>0</v>
+    <row r="24" spans="1:22">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24">
+        <v>0.97</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>7.7700000000000005E-2</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
@@ -889,35 +1240,89 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="13.5">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25">
-        <v>0.96999999999999997</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>2.76E-2</v>
       </c>
       <c r="D25">
-        <v>0.077700000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" ht="13.5">
+        <v>0.1022</v>
+      </c>
+      <c r="E25">
+        <v>67</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>38</v>
       </c>
       <c r="C26">
-        <v>0.0276</v>
+        <v>2.6200000000000001E-2</v>
       </c>
       <c r="D26">
-        <v>0.1022</v>
+        <v>0.10050000000000001</v>
       </c>
       <c r="E26">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -929,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -971,108 +1376,425 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="13.5">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
       </c>
       <c r="C27">
-        <v>0.026200000000000001</v>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="D27">
-        <v>0.10050000000000001</v>
+        <v>9.6100000000000005E-2</v>
       </c>
       <c r="E27">
+        <v>73</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>19</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="B32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32" t="s">
+        <v>12</v>
+      </c>
+      <c r="J32" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" t="s">
+        <v>14</v>
+      </c>
+      <c r="L32" t="s">
+        <v>15</v>
+      </c>
+      <c r="M32" t="s">
+        <v>16</v>
+      </c>
+      <c r="N32" t="s">
+        <v>17</v>
+      </c>
+      <c r="O32" t="s">
+        <v>18</v>
+      </c>
+      <c r="P32" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>20</v>
+      </c>
+      <c r="R32" t="s">
+        <v>21</v>
+      </c>
+      <c r="S32" t="s">
+        <v>22</v>
+      </c>
+      <c r="T32" t="s">
+        <v>23</v>
+      </c>
+      <c r="U32" t="s">
+        <v>24</v>
+      </c>
+      <c r="V32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33">
+        <v>0.97</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>2.93E-2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>29</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="1">
+        <v>44379</v>
+      </c>
+      <c r="K33" t="s">
+        <v>33</v>
+      </c>
+      <c r="L33" t="s">
+        <v>31</v>
+      </c>
+      <c r="M33" t="s">
+        <v>34</v>
+      </c>
+      <c r="N33" t="s">
+        <v>31</v>
+      </c>
+      <c r="O33" t="s">
+        <v>35</v>
+      </c>
+      <c r="P33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>44413</v>
+      </c>
+      <c r="R33" t="s">
+        <v>31</v>
+      </c>
+      <c r="S33" s="1">
+        <v>44258</v>
+      </c>
+      <c r="T33">
+        <v>91</v>
+      </c>
+      <c r="U33" s="1">
+        <v>44319</v>
+      </c>
+      <c r="V33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>1.4460000000000001E-2</v>
+      </c>
+      <c r="D34">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="E34">
+        <v>67</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>9</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35">
+        <v>1.3650000000000001E-2</v>
+      </c>
+      <c r="D35">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="E35">
         <v>68</v>
       </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
         <v>17</v>
       </c>
-      <c r="J27">
-        <v>0</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" ht="13.5">
-      <c r="A28" t="s">
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B36" t="s">
         <v>38</v>
       </c>
-      <c r="C28">
-        <v>0.027199999999999998</v>
-      </c>
-      <c r="D28">
-        <v>0.096100000000000005</v>
-      </c>
-      <c r="E28">
+      <c r="C36">
+        <v>1.3610000000000001E-2</v>
+      </c>
+      <c r="D36">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E36">
         <v>73</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
         <v>19</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>0</v>
+      </c>
+      <c r="T36">
+        <v>0</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+      <c r="V36">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
-  <printOptions/>
   <pageMargins left="1" right="1" top="1.6666666666666667" bottom="1.6666666666666667" header="1" footer="1"/>
-  <pageSetup blackAndWhite="0" cellComments="asDisplayed" draft="0" errors="displayed" fitToHeight="0" fitToWidth="0" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="0"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" cellComments="asDisplayed"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>